<commit_message>
Implemented PCA analysis for metrics.
</commit_message>
<xml_diff>
--- a/result/metrics_values/mall-swarm.xlsx
+++ b/result/metrics_values/mall-swarm.xlsx
@@ -865,7 +865,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.0001615282395774265</t>
+          <t>0.00035452520676794214</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1484,7 +1484,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>8.683520220749258e-05</t>
+          <t>6.700674667422045e-05</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0006464556593960166</t>
+          <t>0.0006045374836750239</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>8.87314347097146e-05</t>
+          <t>0.00011287540173595389</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">

</xml_diff>